<commit_message>
Fix y-labels by manually rotating 90 degree.
</commit_message>
<xml_diff>
--- a/FigureData.xlsx
+++ b/FigureData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>x-labels</t>
   </si>
@@ -34,10 +34,10 @@
     <t>y-text</t>
   </si>
   <si>
-    <t>SPL</t>
-  </si>
-  <si>
-    <t>(3M)</t>
+    <t>‘Yields</t>
+  </si>
+  <si>
+    <t>(wt'/o)</t>
   </si>
   <si>
     <t>y-labels</t>
@@ -64,24 +64,24 @@
     <t>legends</t>
   </si>
   <si>
+    <t>product_™</t>
+  </si>
+  <si>
+    <t>Gaseous</t>
+  </si>
+  <si>
+    <t>Solid_®</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>Bio-o1l_B</t>
+  </si>
+  <si>
     <t>Aqueous</t>
   </si>
   <si>
-    <t>Solid_®</t>
-  </si>
-  <si>
-    <t>Bio-o1l_B</t>
-  </si>
-  <si>
-    <t>product_™</t>
-  </si>
-  <si>
-    <t>Gaseous</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>1toS</t>
   </si>
   <si>
@@ -121,13 +121,13 @@
     <t>50</t>
   </si>
   <si>
-    <t>‘spunodutos</t>
-  </si>
-  <si>
-    <t>Aouanbaay</t>
-  </si>
-  <si>
-    <t>jo</t>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>compounds</t>
   </si>
   <si>
     <t>45</t>
@@ -163,10 +163,7 @@
     <t>360</t>
   </si>
   <si>
-    <t>PPA,</t>
-  </si>
-  <si>
-    <t>(%1M)</t>
+    <t>Yield(wt%)</t>
   </si>
   <si>
     <t>100</t>
@@ -178,24 +175,24 @@
     <t>60</t>
   </si>
   <si>
+    <t>HON</t>
+  </si>
+  <si>
+    <t>he</t>
+  </si>
+  <si>
     <t>NO</t>
   </si>
   <si>
-    <t>he</t>
+    <t>iy</t>
+  </si>
+  <si>
+    <t>Ag</t>
   </si>
   <si>
     <t>EY</t>
   </si>
   <si>
-    <t>Ag</t>
-  </si>
-  <si>
-    <t>HON</t>
-  </si>
-  <si>
-    <t>iy</t>
-  </si>
-  <si>
     <t>230</t>
   </si>
   <si>
@@ -217,13 +214,13 @@
     <t>290</t>
   </si>
   <si>
+    <t>Yield</t>
+  </si>
+  <si>
     <t>(%)</t>
   </si>
   <si>
-    <t>PIPLA</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>_</t>
   </si>
   <si>
     <t>00</t>
@@ -232,16 +229,16 @@
     <t>BO</t>
   </si>
   <si>
+    <t>HS</t>
+  </si>
+  <si>
     <t>GA</t>
   </si>
   <si>
+    <t>[i</t>
+  </si>
+  <si>
     <t>SRL</t>
-  </si>
-  <si>
-    <t>HS</t>
-  </si>
-  <si>
-    <t>[i</t>
   </si>
 </sst>
 </file>
@@ -812,15 +809,15 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
         <f/>
         <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -1006,22 +1003,19 @@
       <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -1038,22 +1032,22 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>57</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1075,25 +1069,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1101,13 +1095,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1115,13 +1109,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
@@ -1138,19 +1132,19 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>73</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add caption data in excel sheet.
</commit_message>
<xml_diff>
--- a/FigureData.xlsx
+++ b/FigureData.xlsx
@@ -17,7 +17,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>Fig. 1. Yields of product fractions produced from the HTL process of the four crop straws.</t>
+  </si>
   <si>
     <t>x-labels</t>
   </si>
@@ -25,6 +31,9 @@
     <t>cs</t>
   </si>
   <si>
+    <t>PS</t>
+  </si>
+  <si>
     <t>RS</t>
   </si>
   <si>
@@ -64,31 +73,37 @@
     <t>legends</t>
   </si>
   <si>
-    <t>product_™</t>
-  </si>
-  <si>
-    <t>Gaseous</t>
-  </si>
-  <si>
-    <t>Solid_®</t>
-  </si>
-  <si>
     <t>product</t>
   </si>
   <si>
-    <t>Bio-o1l_B</t>
+    <t>COU</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>PLOGUCT</t>
   </si>
   <si>
     <t>Aqueous</t>
   </si>
   <si>
-    <t>1toS</t>
+    <t>Gi</t>
+  </si>
+  <si>
+    <t>Bio-oll</t>
+  </si>
+  <si>
+    <t>Fig. 8. Segregation of compounds on the basis of carbon numbers in the biocrude obtained after hydrothermal liquefaction of algal biomass cultivated in wastewater.</t>
+  </si>
+  <si>
+    <t>105</t>
   </si>
   <si>
     <t>Gtol0</t>
   </si>
   <si>
-    <t>11</t>
+    <t>1</t>
   </si>
   <si>
     <t>to</t>
@@ -103,21 +118,24 @@
     <t>20</t>
   </si>
   <si>
-    <t>21</t>
+    <t>24</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>26</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
+    <t>40</t>
+  </si>
+  <si>
     <t>41</t>
   </si>
   <si>
+    <t>C0</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
@@ -133,9 +151,6 @@
     <t>45</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -151,15 +166,27 @@
     <t>0</t>
   </si>
   <si>
+    <t>Fig. 2. Effect of solvents on the products yields ( : Aqueous fraction; : Gases; : Bio-oil; : Solid residue) of WSSliquefied in (a) MeOH–H2O and (b) HEX-H2O for 20min as a function of the temperature.</t>
+  </si>
+  <si>
+    <t>300)</t>
+  </si>
+  <si>
+    <t>320)</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>360)</t>
+  </si>
+  <si>
     <t>300</t>
   </si>
   <si>
     <t>320</t>
   </si>
   <si>
-    <t>340</t>
-  </si>
-  <si>
     <t>360</t>
   </si>
   <si>
@@ -175,28 +202,19 @@
     <t>60</t>
   </si>
   <si>
-    <t>HON</t>
-  </si>
-  <si>
-    <t>he</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>iy</t>
-  </si>
-  <si>
-    <t>Ag</t>
-  </si>
-  <si>
-    <t>EY</t>
+    <t>(a)</t>
+  </si>
+  <si>
+    <t>(by</t>
+  </si>
+  <si>
+    <t>Fig. 1 shows the effect of the reaction temperature on the yields of products and all the experiments were carried out at 30min holding time, with an algae/water of 1/4 and a catalyst aldosage of 5 wt%. The reaction temperature varied from 230 to 290 °C below the critical point of water (374 °C). Initially only 34.15 wt% of bio-oil yield was obtained at 230 °C due to the incomplete degradation of algae at lower temperature stage. As reaction temperature increased, the cleavage of chemical bonds facilitated the decomposition of biomass and a peak of 43.05 wt% appeared at 260 °C, suggesting that hydrolysis reaction of compounds was accelerated and became predominant (Muppaneni et al., 2017). At lower temperature stage, the ionic product (Kw= [H+] [OH−]) of water increased and released more H+ and OH− ion, which showed a stronger capability to hydrolyze more biochemical</t>
   </si>
   <si>
     <t>230</t>
   </si>
   <si>
-    <t>240,</t>
+    <t>240)</t>
   </si>
   <si>
     <t>250</t>
@@ -226,19 +244,16 @@
     <t>00</t>
   </si>
   <si>
-    <t>BO</t>
-  </si>
-  <si>
-    <t>HS</t>
+    <t>RO</t>
   </si>
   <si>
     <t>GA</t>
   </si>
   <si>
-    <t>[i</t>
-  </si>
-  <si>
-    <t>SRL</t>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>SR</t>
   </si>
 </sst>
 </file>
@@ -296,9 +311,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>307925</xdr:colOff>
+      <xdr:colOff>303086</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>38933</xdr:rowOff>
+      <xdr:rowOff>37643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -316,7 +331,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="1333500"/>
-          <a:ext cx="13719125" cy="3658433"/>
+          <a:ext cx="13714286" cy="3657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -339,9 +354,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>307925</xdr:colOff>
+      <xdr:colOff>303086</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>38933</xdr:rowOff>
+      <xdr:rowOff>37643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -359,7 +374,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="1333500"/>
-          <a:ext cx="13719125" cy="3658433"/>
+          <a:ext cx="13714286" cy="3657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -382,9 +397,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>307925</xdr:colOff>
+      <xdr:colOff>303086</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>38933</xdr:rowOff>
+      <xdr:rowOff>37643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -402,7 +417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="1333500"/>
-          <a:ext cx="13719125" cy="3658433"/>
+          <a:ext cx="13714286" cy="3657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -425,9 +440,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>307925</xdr:colOff>
+      <xdr:colOff>303086</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>38933</xdr:rowOff>
+      <xdr:rowOff>37643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -445,7 +460,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="1333500"/>
-          <a:ext cx="13719125" cy="3658433"/>
+          <a:ext cx="13714286" cy="3657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -742,7 +757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -755,21 +770,21 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -783,44 +798,54 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="G4">
-        <f/>
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D5" t="s">
         <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -831,126 +856,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="J2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -961,7 +994,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -972,36 +1005,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1009,45 +1042,41 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1058,7 +1087,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1069,39 +1098,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
         <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1109,42 +1132,53 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>